<commit_message>
Menambahkan file tugas vlookup hlookup
</commit_message>
<xml_diff>
--- a/MATERIALPRAKERIN-main/mail merge.xlsx
+++ b/MATERIALPRAKERIN-main/mail merge.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRAKERIN\2024\MATERIALPRAKERIN-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -486,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L17"/>
+  <dimension ref="A2:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,12 +501,14 @@
     <col min="5" max="5" width="33.42578125" style="1" customWidth="1"/>
     <col min="6" max="7" width="13.140625" style="1" customWidth="1"/>
     <col min="8" max="9" width="13" style="1" customWidth="1"/>
-    <col min="10" max="11" width="13.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="32.7109375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="13" max="13" width="25.5703125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -540,8 +542,14 @@
       <c r="K2" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="L2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -579,8 +587,14 @@
         <f>IF(AND(J3&gt;86,J3&lt;=100),"A (Memuaskan)",IF(AND(J3&gt;75,J3&lt;=85),"B (Baik)",IF(AND(J3&gt;=60,J3&lt;=74),"C (Kurang)",IF(AND(J3&gt;=0,J3&lt;=59),"D (Tidak lulus)"))))</f>
         <v>A (Memuaskan)</v>
       </c>
+      <c r="L3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -615,11 +629,17 @@
         <v>89</v>
       </c>
       <c r="K4" s="1" t="str">
-        <f t="shared" ref="K4:K7" si="2">IF(AND(J4&gt;86,J4&lt;=100),"A (Memuaskan)",IF(AND(J4&gt;75,J4&lt;=85),"B (Baik)",IF(AND(J4&gt;=60,J4&lt;=74),"C (Kurang)",IF(AND(J4&gt;=0,J4&lt;=59),"D (Tidak lulus)"))))</f>
+        <f>IF(AND(J4&gt;86,J4&lt;=100),"A (Memuaskan)",IF(AND(J4&gt;75,J4&lt;=85),"B (Baik)",IF(AND(J4&gt;=60,J4&lt;=74),"C (Kurang)",IF(AND(J4&gt;=0,J4&lt;=59),"D (Tidak lulus)"))))</f>
         <v>A (Memuaskan)</v>
       </c>
+      <c r="L4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -639,7 +659,7 @@
         <v>89</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" ref="G5:G7" si="3">F5*0.7</f>
+        <f t="shared" ref="G5:G7" si="2">F5*0.7</f>
         <v>62.3</v>
       </c>
       <c r="H5" s="2">
@@ -654,11 +674,17 @@
         <v>89</v>
       </c>
       <c r="K5" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K4:K7" si="3">IF(AND(J5&gt;86,J5&lt;=100),"A (Memuaskan)",IF(AND(J5&gt;75,J5&lt;=85),"B (Baik)",IF(AND(J5&gt;=60,J5&lt;=74),"C (Kurang)",IF(AND(J5&gt;=0,J5&lt;=59),"D (Tidak lulus)"))))</f>
         <v>A (Memuaskan)</v>
       </c>
+      <c r="L5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -678,7 +704,7 @@
         <v>89</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>62.3</v>
       </c>
       <c r="H6" s="2">
@@ -693,11 +719,17 @@
         <v>89</v>
       </c>
       <c r="K6" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>A (Memuaskan)</v>
       </c>
+      <c r="L6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -717,7 +749,7 @@
         <v>89</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>62.3</v>
       </c>
       <c r="H7" s="2">
@@ -732,55 +764,13 @@
         <v>89</v>
       </c>
       <c r="K7" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>A (Memuaskan)</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K13" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L13" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K17" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L17" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>